<commit_message>
Added shell script to run analyse script.
</commit_message>
<xml_diff>
--- a/data/Amino acid occurence.xlsx
+++ b/data/Amino acid occurence.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300"/>
+    <workbookView xWindow="720" yWindow="400" windowWidth="27560" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -504,12 +507,12 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="20" width="9.140625" style="1"/>
+    <col min="1" max="20" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="5" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -571,7 +574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -633,7 +636,7 @@
         <v>6.0377358490566042</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -695,7 +698,7 @@
         <v>2.2641509433962264</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -757,7 +760,7 @@
         <v>7.9245283018867925</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -819,7 +822,7 @@
         <v>6.7924528301886795</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -881,7 +884,7 @@
         <v>9.0566037735849054</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -943,7 +946,7 @@
         <v>0.75471698113207553</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>13.962264150943396</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>17.735849056603772</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>9.433962264150944</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>6.4150943396226419</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1253,7 +1256,7 @@
         <v>8.6792452830188669</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>10.943396226415095</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20">
       <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
@@ -1368,7 +1371,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
@@ -1423,29 +1426,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>